<commit_message>
add missing MATLAB result columns
</commit_message>
<xml_diff>
--- a/exposan/bsm1/results/matlab_exported_data.xlsx
+++ b/exposan/bsm1/results/matlab_exported_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Research/Modeling/MATLAB/bsm1_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bsm1/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{AA39BFF5-B466-4BE5-BF90-088EEF79C798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCCF2C79-E94B-4AFA-B638-3B8E6A970604}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{AA39BFF5-B466-4BE5-BF90-088EEF79C798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DAD77C4-61C0-EA48-867F-4C797A8C5389}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="11250" xr2:uid="{03E94F00-A3DB-478B-94D3-87D7A3CD8B7E}"/>
+    <workbookView xWindow="6140" yWindow="1700" windowWidth="26520" windowHeight="14220" xr2:uid="{03E94F00-A3DB-478B-94D3-87D7A3CD8B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -33,8 +33,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yalin Li</author>
+  </authors>
+  <commentList>
+    <comment ref="DS2" authorId="0" shapeId="0" xr:uid="{5B1A088F-9803-2549-8528-D57B1098D1C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yalin Li:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TSS10/TSSin</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DT2" authorId="0" shapeId="0" xr:uid="{1A1884C3-326A-5D40-9BF7-02A5CB9B5873}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yalin Li:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TSS1/TSSin</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="108">
   <si>
     <t>t</t>
   </si>
@@ -139,9 +215,6 @@
   </si>
   <si>
     <t>Qe</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
   <si>
     <t>SI1</t>
@@ -356,18 +429,37 @@
   <si>
     <t>TSS</t>
   </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>gamma_eff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -781,19 +873,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F83A2F-FEC5-49DE-AE7D-BD2A3885C2C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F83A2F-FEC5-49DE-AE7D-BD2A3885C2C9}">
   <dimension ref="A1:GL53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="DK3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomRight" activeCell="DT2" sqref="DT2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1095,7 @@
       <c r="GK1" s="3"/>
       <c r="GL1" s="3"/>
     </row>
-    <row r="2" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1317,7 +1409,7 @@
         <v>13</v>
       </c>
       <c r="DG2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="DH2" s="1" t="s">
         <v>34</v>
@@ -1353,223 +1445,223 @@
         <v>25</v>
       </c>
       <c r="DS2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DT2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DU2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="DT2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="DU2" s="1" t="s">
+      <c r="DV2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="DV2" s="1" t="s">
+      <c r="DW2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="DW2" s="1" t="s">
+      <c r="DX2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="DX2" s="1" t="s">
+      <c r="DY2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DY2" s="1" t="s">
+      <c r="DZ2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DZ2" s="1" t="s">
+      <c r="EA2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="EA2" s="1" t="s">
+      <c r="EB2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="EB2" s="1" t="s">
+      <c r="EC2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="EC2" s="1" t="s">
+      <c r="ED2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="ED2" s="1" t="s">
+      <c r="EE2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="EE2" s="1" t="s">
+      <c r="EF2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="EF2" s="1" t="s">
+      <c r="EG2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="EG2" s="1" t="s">
+      <c r="EH2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="EH2" s="1" t="s">
+      <c r="EI2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="EI2" s="1" t="s">
+      <c r="EJ2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="EJ2" s="1" t="s">
+      <c r="EK2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="EK2" s="1" t="s">
+      <c r="EL2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="EL2" s="1" t="s">
+      <c r="EM2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="EM2" s="1" t="s">
+      <c r="EN2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="EN2" s="1" t="s">
+      <c r="EO2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="EO2" s="1" t="s">
+      <c r="EP2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="EP2" s="1" t="s">
+      <c r="EQ2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="EQ2" s="1" t="s">
+      <c r="ER2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="ER2" s="1" t="s">
+      <c r="ES2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="ES2" s="1" t="s">
+      <c r="ET2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="ET2" s="1" t="s">
+      <c r="EU2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="EU2" s="1" t="s">
+      <c r="EV2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="EV2" s="1" t="s">
+      <c r="EW2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="EW2" s="1" t="s">
+      <c r="EX2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="EX2" s="1" t="s">
+      <c r="EY2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="EY2" s="1" t="s">
+      <c r="EZ2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="EZ2" s="1" t="s">
+      <c r="FA2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="FA2" s="1" t="s">
+      <c r="FB2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="FB2" s="1" t="s">
+      <c r="FC2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="FC2" s="1" t="s">
+      <c r="FD2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="FD2" s="1" t="s">
+      <c r="FE2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="FE2" s="1" t="s">
+      <c r="FF2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="FF2" s="1" t="s">
+      <c r="FG2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="FG2" s="1" t="s">
+      <c r="FH2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="FH2" s="1" t="s">
+      <c r="FI2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="FI2" s="1" t="s">
+      <c r="FJ2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="FJ2" s="1" t="s">
+      <c r="FK2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="FK2" s="1" t="s">
+      <c r="FL2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="FL2" s="1" t="s">
+      <c r="FM2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="FM2" s="1" t="s">
+      <c r="FN2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="FN2" s="1" t="s">
+      <c r="FO2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="FO2" s="1" t="s">
+      <c r="FP2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="FP2" s="1" t="s">
+      <c r="FQ2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="FQ2" s="1" t="s">
+      <c r="FR2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="FR2" s="1" t="s">
+      <c r="FS2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="FS2" s="1" t="s">
+      <c r="FT2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="FT2" s="1" t="s">
+      <c r="FU2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="FU2" s="1" t="s">
+      <c r="FV2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="FV2" s="1" t="s">
+      <c r="FW2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="FW2" s="1" t="s">
+      <c r="FX2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="FX2" s="1" t="s">
+      <c r="FY2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="FY2" s="1" t="s">
+      <c r="FZ2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="FZ2" s="1" t="s">
+      <c r="GA2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="GA2" s="1" t="s">
+      <c r="GB2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="GB2" s="1" t="s">
+      <c r="GC2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="GC2" s="1" t="s">
+      <c r="GD2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="GD2" s="1" t="s">
+      <c r="GE2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="GE2" s="1" t="s">
+      <c r="GF2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="GF2" s="1" t="s">
+      <c r="GG2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="GG2" s="1" t="s">
+      <c r="GH2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="GH2" s="1" t="s">
+      <c r="GI2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="GI2" s="1" t="s">
+      <c r="GJ2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="GJ2" s="1" t="s">
+      <c r="GK2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="GK2" s="1" t="s">
+      <c r="GL2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="GL2" s="1" t="s">
-        <v>105</v>
-      </c>
     </row>
-    <row r="3" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2138,7 +2230,7 @@
         <v>4.1256000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2707,7 +2799,7 @@
         <v>3.8678956457825402</v>
       </c>
     </row>
-    <row r="5" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3276,7 +3368,7 @@
         <v>4.26338721014484</v>
       </c>
     </row>
-    <row r="6" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3845,7 +3937,7 @@
         <v>4.4220118942718702</v>
       </c>
     </row>
-    <row r="7" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4414,7 +4506,7 @@
         <v>4.49608229692174</v>
       </c>
     </row>
-    <row r="8" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4983,7 +5075,7 @@
         <v>4.5270516530330802</v>
       </c>
     </row>
-    <row r="9" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -5552,7 +5644,7 @@
         <v>4.5325202450545197</v>
       </c>
     </row>
-    <row r="10" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -6121,7 +6213,7 @@
         <v>4.5221980584568104</v>
       </c>
     </row>
-    <row r="11" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -6690,7 +6782,7 @@
         <v>4.5021765721988496</v>
       </c>
     </row>
-    <row r="12" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -7259,7 +7351,7 @@
         <v>4.4765317953873502</v>
       </c>
     </row>
-    <row r="13" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -7828,7 +7920,7 @@
         <v>4.4480704062508796</v>
       </c>
     </row>
-    <row r="14" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -8397,7 +8489,7 @@
         <v>4.4187370818248501</v>
       </c>
     </row>
-    <row r="15" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -8966,7 +9058,7 @@
         <v>4.3898574639790002</v>
       </c>
     </row>
-    <row r="16" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -9535,7 +9627,7 @@
         <v>4.3622865873588603</v>
       </c>
     </row>
-    <row r="17" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -10104,7 +10196,7 @@
         <v>4.3365384703303702</v>
       </c>
     </row>
-    <row r="18" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -10673,7 +10765,7 @@
         <v>4.31288943532111</v>
       </c>
     </row>
-    <row r="19" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -11242,7 +11334,7 @@
         <v>4.2914300704875004</v>
       </c>
     </row>
-    <row r="20" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -11811,7 +11903,7 @@
         <v>4.2721338007865501</v>
       </c>
     </row>
-    <row r="21" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -12380,7 +12472,7 @@
         <v>4.2548990706819403</v>
       </c>
     </row>
-    <row r="22" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -12949,7 +13041,7 @@
         <v>4.2395807793926501</v>
       </c>
     </row>
-    <row r="23" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -13518,7 +13610,7 @@
         <v>4.2260136667338601</v>
       </c>
     </row>
-    <row r="24" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -14087,7 +14179,7 @@
         <v>4.2140272714548797</v>
       </c>
     </row>
-    <row r="25" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -14656,7 +14748,7 @@
         <v>4.20345594681406</v>
       </c>
     </row>
-    <row r="26" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -15225,7 +15317,7 @@
         <v>4.1941430987239103</v>
       </c>
     </row>
-    <row r="27" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -15794,7 +15886,7 @@
         <v>4.1859446703647603</v>
       </c>
     </row>
-    <row r="28" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -16363,7 +16455,7 @@
         <v>4.1787308771020104</v>
       </c>
     </row>
-    <row r="29" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -16932,7 +17024,7 @@
         <v>4.1723847993353003</v>
       </c>
     </row>
-    <row r="30" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -17501,7 +17593,7 @@
         <v>4.1668023357328403</v>
       </c>
     </row>
-    <row r="31" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -18070,7 +18162,7 @@
         <v>4.1618903011351298</v>
       </c>
     </row>
-    <row r="32" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -18639,7 +18731,7 @@
         <v>4.1575692155921002</v>
       </c>
     </row>
-    <row r="33" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -19208,7 +19300,7 @@
         <v>4.1537673013638798</v>
       </c>
     </row>
-    <row r="34" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -19777,7 +19869,7 @@
         <v>4.1504213468045297</v>
       </c>
     </row>
-    <row r="35" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>32</v>
       </c>
@@ -20346,7 +20438,7 @@
         <v>4.1474763981649598</v>
       </c>
     </row>
-    <row r="36" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>33</v>
       </c>
@@ -20915,7 +21007,7 @@
         <v>4.1448842617777402</v>
       </c>
     </row>
-    <row r="37" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>34</v>
       </c>
@@ -21484,7 +21576,7 @@
         <v>4.1426018233537603</v>
       </c>
     </row>
-    <row r="38" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>35</v>
       </c>
@@ -22053,7 +22145,7 @@
         <v>4.1405915374954603</v>
       </c>
     </row>
-    <row r="39" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>36</v>
       </c>
@@ -22622,7 +22714,7 @@
         <v>4.1388207722126902</v>
       </c>
     </row>
-    <row r="40" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>37</v>
       </c>
@@ -23191,7 +23283,7 @@
         <v>4.1372606976570498</v>
       </c>
     </row>
-    <row r="41" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>38</v>
       </c>
@@ -23760,7 +23852,7 @@
         <v>4.1358859824018204</v>
       </c>
     </row>
-    <row r="42" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>39</v>
       </c>
@@ -24329,7 +24421,7 @@
         <v>4.1346744003113898</v>
       </c>
     </row>
-    <row r="43" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -24898,7 +24990,7 @@
         <v>4.1336064167293598</v>
       </c>
     </row>
-    <row r="44" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>41</v>
       </c>
@@ -25467,7 +25559,7 @@
         <v>4.1326648574620997</v>
       </c>
     </row>
-    <row r="45" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>42</v>
       </c>
@@ -26036,7 +26128,7 @@
         <v>4.1318342492940197</v>
       </c>
     </row>
-    <row r="46" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>43</v>
       </c>
@@ -26605,7 +26697,7 @@
         <v>4.1311017819985798</v>
       </c>
     </row>
-    <row r="47" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>44</v>
       </c>
@@ -27174,7 +27266,7 @@
         <v>4.1304556523906202</v>
       </c>
     </row>
-    <row r="48" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>45</v>
       </c>
@@ -27743,7 +27835,7 @@
         <v>4.1298858763502704</v>
       </c>
     </row>
-    <row r="49" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>46</v>
       </c>
@@ -28312,7 +28404,7 @@
         <v>4.1293832124474701</v>
       </c>
     </row>
-    <row r="50" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>47</v>
       </c>
@@ -28881,7 +28973,7 @@
         <v>4.1289395992460802</v>
       </c>
     </row>
-    <row r="51" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>48</v>
       </c>
@@ -29450,7 +29542,7 @@
         <v>4.1285480909255403</v>
       </c>
     </row>
-    <row r="52" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>49</v>
       </c>
@@ -30019,7 +30111,7 @@
         <v>4.1282026309168796</v>
       </c>
     </row>
-    <row r="53" spans="1:194" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>50</v>
       </c>
@@ -30633,5 +30725,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add functions for convenient simulation with different initial conditions
</commit_message>
<xml_diff>
--- a/exposan/bsm1/results/matlab_exported_data.xlsx
+++ b/exposan/bsm1/results/matlab_exported_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bsm1/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\bsm1\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{AA39BFF5-B466-4BE5-BF90-088EEF79C798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DAD77C4-61C0-EA48-867F-4C797A8C5389}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BB8DCE-ABC8-43A6-8039-6B19502B581A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="1700" windowWidth="26520" windowHeight="14220" xr2:uid="{03E94F00-A3DB-478B-94D3-87D7A3CD8B7E}"/>
+    <workbookView xWindow="-14340" yWindow="1650" windowWidth="11580" windowHeight="9150" xr2:uid="{03E94F00-A3DB-478B-94D3-87D7A3CD8B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="107">
   <si>
     <t>t</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>S_ALK</t>
-  </si>
-  <si>
-    <t>S_N2</t>
   </si>
   <si>
     <t>Q</t>
@@ -877,20 +874,20 @@
   <dimension ref="A1:GL53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="DK3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="BN3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DT2" sqref="DT2"/>
+      <selection pane="bottomRight" activeCell="BT31" sqref="BT31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -908,7 +905,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
@@ -926,7 +923,7 @@
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
       <c r="AH1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
@@ -944,7 +941,7 @@
       <c r="AV1" s="3"/>
       <c r="AW1" s="3"/>
       <c r="AX1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
@@ -962,7 +959,7 @@
       <c r="BL1" s="3"/>
       <c r="BM1" s="3"/>
       <c r="BN1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BO1" s="3"/>
       <c r="BP1" s="3"/>
@@ -980,7 +977,7 @@
       <c r="CB1" s="3"/>
       <c r="CC1" s="3"/>
       <c r="CD1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="CE1" s="3"/>
       <c r="CF1" s="3"/>
@@ -1095,7 +1092,7 @@
       <c r="GK1" s="3"/>
       <c r="GL1" s="3"/>
     </row>
-    <row r="2" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:194" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1136,10 +1133,10 @@
         <v>13</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>1</v>
@@ -1181,10 +1178,10 @@
         <v>13</v>
       </c>
       <c r="AE2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>1</v>
@@ -1226,10 +1223,10 @@
         <v>13</v>
       </c>
       <c r="AU2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="AX2" s="1" t="s">
         <v>1</v>
@@ -1271,10 +1268,10 @@
         <v>13</v>
       </c>
       <c r="BK2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="BN2" s="1" t="s">
         <v>1</v>
@@ -1316,10 +1313,10 @@
         <v>13</v>
       </c>
       <c r="CA2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="CB2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="CD2" s="1" t="s">
         <v>1</v>
@@ -1361,13 +1358,13 @@
         <v>13</v>
       </c>
       <c r="CQ2" s="1" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="CR2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CS2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="CS2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="CT2" s="1" t="s">
         <v>1</v>
@@ -1409,259 +1406,259 @@
         <v>13</v>
       </c>
       <c r="DG2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DH2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="DI2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="DJ2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="DK2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="DL2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="DM2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="DN2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="DO2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="DP2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="DQ2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DR2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="DS2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DH2" s="1" t="s">
+      <c r="DT2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DU2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="DI2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="DJ2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="DK2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="DL2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="DM2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="DN2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="DO2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="DP2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="DQ2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="DR2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="DS2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DT2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DU2" s="1" t="s">
+      <c r="DV2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="DV2" s="1" t="s">
+      <c r="DW2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="DW2" s="1" t="s">
+      <c r="DX2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="DX2" s="1" t="s">
+      <c r="DY2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="DY2" s="1" t="s">
+      <c r="DZ2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DZ2" s="1" t="s">
+      <c r="EA2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="EA2" s="1" t="s">
+      <c r="EB2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="EB2" s="1" t="s">
+      <c r="EC2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="EC2" s="1" t="s">
+      <c r="ED2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="ED2" s="1" t="s">
+      <c r="EE2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="EE2" s="1" t="s">
+      <c r="EF2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="EF2" s="1" t="s">
+      <c r="EG2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="EG2" s="1" t="s">
+      <c r="EH2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="EH2" s="1" t="s">
+      <c r="EI2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="EI2" s="1" t="s">
+      <c r="EJ2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="EJ2" s="1" t="s">
+      <c r="EK2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="EK2" s="1" t="s">
+      <c r="EL2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="EL2" s="1" t="s">
+      <c r="EM2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="EM2" s="1" t="s">
+      <c r="EN2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="EN2" s="1" t="s">
+      <c r="EO2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="EO2" s="1" t="s">
+      <c r="EP2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="EP2" s="1" t="s">
+      <c r="EQ2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="EQ2" s="1" t="s">
+      <c r="ER2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="ER2" s="1" t="s">
+      <c r="ES2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="ES2" s="1" t="s">
+      <c r="ET2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="ET2" s="1" t="s">
+      <c r="EU2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="EU2" s="1" t="s">
+      <c r="EV2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="EV2" s="1" t="s">
+      <c r="EW2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="EW2" s="1" t="s">
+      <c r="EX2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="EX2" s="1" t="s">
+      <c r="EY2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="EY2" s="1" t="s">
+      <c r="EZ2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="EZ2" s="1" t="s">
+      <c r="FA2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="FA2" s="1" t="s">
+      <c r="FB2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="FB2" s="1" t="s">
+      <c r="FC2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="FC2" s="1" t="s">
+      <c r="FD2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="FD2" s="1" t="s">
+      <c r="FE2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="FE2" s="1" t="s">
+      <c r="FF2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="FF2" s="1" t="s">
+      <c r="FG2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="FG2" s="1" t="s">
+      <c r="FH2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="FH2" s="1" t="s">
+      <c r="FI2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="FI2" s="1" t="s">
+      <c r="FJ2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="FJ2" s="1" t="s">
+      <c r="FK2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="FK2" s="1" t="s">
+      <c r="FL2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="FL2" s="1" t="s">
+      <c r="FM2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="FM2" s="1" t="s">
+      <c r="FN2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="FN2" s="1" t="s">
+      <c r="FO2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="FO2" s="1" t="s">
+      <c r="FP2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="FP2" s="1" t="s">
+      <c r="FQ2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="FQ2" s="1" t="s">
+      <c r="FR2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="FR2" s="1" t="s">
+      <c r="FS2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="FS2" s="1" t="s">
+      <c r="FT2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="FT2" s="1" t="s">
+      <c r="FU2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="FU2" s="1" t="s">
+      <c r="FV2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="FV2" s="1" t="s">
+      <c r="FW2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="FW2" s="1" t="s">
+      <c r="FX2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="FX2" s="1" t="s">
+      <c r="FY2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="FY2" s="1" t="s">
+      <c r="FZ2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="FZ2" s="1" t="s">
+      <c r="GA2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="GA2" s="1" t="s">
+      <c r="GB2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="GB2" s="1" t="s">
+      <c r="GC2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="GC2" s="1" t="s">
+      <c r="GD2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="GD2" s="1" t="s">
+      <c r="GE2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="GE2" s="1" t="s">
+      <c r="GF2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="GF2" s="1" t="s">
+      <c r="GG2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="GG2" s="1" t="s">
+      <c r="GH2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="GH2" s="1" t="s">
+      <c r="GI2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="GI2" s="1" t="s">
+      <c r="GJ2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="GJ2" s="1" t="s">
+      <c r="GK2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="GK2" s="1" t="s">
+      <c r="GL2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="GL2" s="1" t="s">
-        <v>104</v>
-      </c>
     </row>
-    <row r="3" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>4.1256000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2799,7 +2796,7 @@
         <v>3.8678956457825402</v>
       </c>
     </row>
-    <row r="5" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3368,7 +3365,7 @@
         <v>4.26338721014484</v>
       </c>
     </row>
-    <row r="6" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3937,7 +3934,7 @@
         <v>4.4220118942718702</v>
       </c>
     </row>
-    <row r="7" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4506,7 +4503,7 @@
         <v>4.49608229692174</v>
       </c>
     </row>
-    <row r="8" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -5075,7 +5072,7 @@
         <v>4.5270516530330802</v>
       </c>
     </row>
-    <row r="9" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -5644,7 +5641,7 @@
         <v>4.5325202450545197</v>
       </c>
     </row>
-    <row r="10" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -6213,7 +6210,7 @@
         <v>4.5221980584568104</v>
       </c>
     </row>
-    <row r="11" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -6782,7 +6779,7 @@
         <v>4.5021765721988496</v>
       </c>
     </row>
-    <row r="12" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -7351,7 +7348,7 @@
         <v>4.4765317953873502</v>
       </c>
     </row>
-    <row r="13" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -7920,7 +7917,7 @@
         <v>4.4480704062508796</v>
       </c>
     </row>
-    <row r="14" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -8489,7 +8486,7 @@
         <v>4.4187370818248501</v>
       </c>
     </row>
-    <row r="15" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -9058,7 +9055,7 @@
         <v>4.3898574639790002</v>
       </c>
     </row>
-    <row r="16" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -9627,7 +9624,7 @@
         <v>4.3622865873588603</v>
       </c>
     </row>
-    <row r="17" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -10196,7 +10193,7 @@
         <v>4.3365384703303702</v>
       </c>
     </row>
-    <row r="18" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -10765,7 +10762,7 @@
         <v>4.31288943532111</v>
       </c>
     </row>
-    <row r="19" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -11334,7 +11331,7 @@
         <v>4.2914300704875004</v>
       </c>
     </row>
-    <row r="20" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -11903,7 +11900,7 @@
         <v>4.2721338007865501</v>
       </c>
     </row>
-    <row r="21" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -12472,7 +12469,7 @@
         <v>4.2548990706819403</v>
       </c>
     </row>
-    <row r="22" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -13041,7 +13038,7 @@
         <v>4.2395807793926501</v>
       </c>
     </row>
-    <row r="23" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -13610,7 +13607,7 @@
         <v>4.2260136667338601</v>
       </c>
     </row>
-    <row r="24" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -14179,7 +14176,7 @@
         <v>4.2140272714548797</v>
       </c>
     </row>
-    <row r="25" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -14748,7 +14745,7 @@
         <v>4.20345594681406</v>
       </c>
     </row>
-    <row r="26" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -15317,7 +15314,7 @@
         <v>4.1941430987239103</v>
       </c>
     </row>
-    <row r="27" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -15886,7 +15883,7 @@
         <v>4.1859446703647603</v>
       </c>
     </row>
-    <row r="28" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -16455,7 +16452,7 @@
         <v>4.1787308771020104</v>
       </c>
     </row>
-    <row r="29" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -17024,7 +17021,7 @@
         <v>4.1723847993353003</v>
       </c>
     </row>
-    <row r="30" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -17593,7 +17590,7 @@
         <v>4.1668023357328403</v>
       </c>
     </row>
-    <row r="31" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -18162,7 +18159,7 @@
         <v>4.1618903011351298</v>
       </c>
     </row>
-    <row r="32" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -18731,7 +18728,7 @@
         <v>4.1575692155921002</v>
       </c>
     </row>
-    <row r="33" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -19300,7 +19297,7 @@
         <v>4.1537673013638798</v>
       </c>
     </row>
-    <row r="34" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -19869,7 +19866,7 @@
         <v>4.1504213468045297</v>
       </c>
     </row>
-    <row r="35" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -20438,7 +20435,7 @@
         <v>4.1474763981649598</v>
       </c>
     </row>
-    <row r="36" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -21007,7 +21004,7 @@
         <v>4.1448842617777402</v>
       </c>
     </row>
-    <row r="37" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -21576,7 +21573,7 @@
         <v>4.1426018233537603</v>
       </c>
     </row>
-    <row r="38" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -22145,7 +22142,7 @@
         <v>4.1405915374954603</v>
       </c>
     </row>
-    <row r="39" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -22714,7 +22711,7 @@
         <v>4.1388207722126902</v>
       </c>
     </row>
-    <row r="40" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -23283,7 +23280,7 @@
         <v>4.1372606976570498</v>
       </c>
     </row>
-    <row r="41" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -23852,7 +23849,7 @@
         <v>4.1358859824018204</v>
       </c>
     </row>
-    <row r="42" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -24421,7 +24418,7 @@
         <v>4.1346744003113898</v>
       </c>
     </row>
-    <row r="43" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -24990,7 +24987,7 @@
         <v>4.1336064167293598</v>
       </c>
     </row>
-    <row r="44" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -25559,7 +25556,7 @@
         <v>4.1326648574620997</v>
       </c>
     </row>
-    <row r="45" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -26128,7 +26125,7 @@
         <v>4.1318342492940197</v>
       </c>
     </row>
-    <row r="46" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -26697,7 +26694,7 @@
         <v>4.1311017819985798</v>
       </c>
     </row>
-    <row r="47" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -27266,7 +27263,7 @@
         <v>4.1304556523906202</v>
       </c>
     </row>
-    <row r="48" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
@@ -27835,7 +27832,7 @@
         <v>4.1298858763502704</v>
       </c>
     </row>
-    <row r="49" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>46</v>
       </c>
@@ -28404,7 +28401,7 @@
         <v>4.1293832124474701</v>
       </c>
     </row>
-    <row r="50" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>47</v>
       </c>
@@ -28973,7 +28970,7 @@
         <v>4.1289395992460802</v>
       </c>
     </row>
-    <row r="51" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48</v>
       </c>
@@ -29542,7 +29539,7 @@
         <v>4.1285480909255403</v>
       </c>
     </row>
-    <row r="52" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
@@ -30111,7 +30108,7 @@
         <v>4.1282026309168796</v>
       </c>
     </row>
-    <row r="53" spans="1:194" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:194" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>50</v>
       </c>

</xml_diff>